<commit_message>
Chnage in FP 8
</commit_message>
<xml_diff>
--- a/result_fp16/meta-llama/Meta-Llama-3-70B.xlsx
+++ b/result_fp16/meta-llama/Meta-Llama-3-70B.xlsx
@@ -1460,85 +1460,85 @@
         <v>0</v>
       </c>
       <c r="H10" t="n">
-        <v>926374</v>
+        <v>935547</v>
       </c>
       <c r="I10" t="n">
-        <v>0.552693</v>
+        <v>0.547273</v>
       </c>
       <c r="J10" t="n">
-        <v>1131.91</v>
+        <v>1120.82</v>
       </c>
       <c r="K10" t="n">
-        <v>57898.1</v>
+        <v>58471.5</v>
       </c>
       <c r="L10" t="n">
-        <v>58060.2</v>
+        <v>58630.6</v>
       </c>
       <c r="M10" t="n">
-        <v>57684.4</v>
+        <v>58294.1</v>
       </c>
       <c r="N10" t="n">
-        <v>58060.2</v>
+        <v>58630.5</v>
       </c>
       <c r="O10" t="n">
-        <v>58023.9</v>
+        <v>58607.9</v>
       </c>
       <c r="P10" t="n">
-        <v>57901</v>
+        <v>58460.6</v>
       </c>
       <c r="Q10" t="n">
-        <v>508.163</v>
+        <v>533.979</v>
       </c>
       <c r="R10" t="n">
-        <v>572.115</v>
+        <v>676.494</v>
       </c>
       <c r="S10" t="n">
-        <v>104.133</v>
+        <v>114.793</v>
       </c>
       <c r="T10" t="n">
-        <v>572.102</v>
+        <v>676.487</v>
       </c>
       <c r="U10" t="n">
-        <v>539.783</v>
+        <v>565.553</v>
       </c>
       <c r="V10" t="n">
-        <v>531.878</v>
+        <v>543.141</v>
       </c>
       <c r="W10" t="n">
-        <v>28.0361</v>
+        <v>28.3036</v>
       </c>
       <c r="X10" t="n">
-        <v>28.2949</v>
+        <v>28.575</v>
       </c>
       <c r="Y10" t="n">
-        <v>27.9275</v>
+        <v>28.2279</v>
       </c>
       <c r="Z10" t="n">
-        <v>28.2914</v>
+        <v>28.5428</v>
       </c>
       <c r="AA10" t="n">
-        <v>28.0841</v>
+        <v>28.3525</v>
       </c>
       <c r="AB10" t="n">
-        <v>28.0482</v>
+        <v>28.3117</v>
       </c>
       <c r="AC10" t="n">
         <v>0</v>
       </c>
       <c r="AD10" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="AE10" t="n">
-        <v>0</v>
+        <v>92.02569444444444</v>
       </c>
       <c r="AF10" t="n">
         <v>0.0006955505630481</v>
       </c>
       <c r="AG10" t="n">
-        <v>0.0027822022521927</v>
+        <v>97.31447927607095</v>
       </c>
       <c r="AH10" t="n">
-        <v>0.0019127640483824</v>
+        <v>91.30805528699688</v>
       </c>
     </row>
     <row r="11">

</xml_diff>

<commit_message>
minor chnage + results
</commit_message>
<xml_diff>
--- a/result_fp16/meta-llama/Meta-Llama-3-70B.xlsx
+++ b/result_fp16/meta-llama/Meta-Llama-3-70B.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AH1"/>
+  <dimension ref="A1:AH2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -605,6 +605,110 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>130</v>
+      </c>
+      <c r="B2" t="n">
+        <v>2048</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1024</v>
+      </c>
+      <c r="D2" t="n">
+        <v>8</v>
+      </c>
+      <c r="E2" t="n">
+        <v>8</v>
+      </c>
+      <c r="F2" t="n">
+        <v>1024</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" t="n">
+        <v>3712360</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.275835</v>
+      </c>
+      <c r="J2" t="n">
+        <v>564.91</v>
+      </c>
+      <c r="K2" t="n">
+        <v>29002.7</v>
+      </c>
+      <c r="L2" t="n">
+        <v>29032.1</v>
+      </c>
+      <c r="M2" t="n">
+        <v>28934.4</v>
+      </c>
+      <c r="N2" t="n">
+        <v>29025.2</v>
+      </c>
+      <c r="O2" t="n">
+        <v>29020.5</v>
+      </c>
+      <c r="P2" t="n">
+        <v>29009.7</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>77.401</v>
+      </c>
+      <c r="R2" t="n">
+        <v>95.2076</v>
+      </c>
+      <c r="S2" t="n">
+        <v>47.7616</v>
+      </c>
+      <c r="T2" t="n">
+        <v>94.797</v>
+      </c>
+      <c r="U2" t="n">
+        <v>93.9948</v>
+      </c>
+      <c r="V2" t="n">
+        <v>63.1103</v>
+      </c>
+      <c r="W2" t="n">
+        <v>14.1306</v>
+      </c>
+      <c r="X2" t="n">
+        <v>14.153</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>14.0892</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>14.1495</v>
+      </c>
+      <c r="AA2" t="n">
+        <v>14.146</v>
+      </c>
+      <c r="AB2" t="n">
+        <v>14.1304</v>
+      </c>
+      <c r="AC2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD2" t="n">
+        <v>100</v>
+      </c>
+      <c r="AE2" t="n">
+        <v>97.20871845005333</v>
+      </c>
+      <c r="AF2" t="n">
+        <v>0.0006955505630481</v>
+      </c>
+      <c r="AG2" t="n">
+        <v>95.8941650263266</v>
+      </c>
+      <c r="AH2" t="n">
+        <v>94.62826195070886</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>